<commit_message>
properties and file names changed
</commit_message>
<xml_diff>
--- a/ddf--list--geo--global.xlsx
+++ b/ddf--list--geo--global.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ola\Documents\GitHub\ddf_xlsx--gapminder--geo_countries_and_groups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ola\Documents\GitHub\ddf--gapminder--geo_countries_and_groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,14 +71,6 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,12 +304,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -545,18 +533,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="_e_geo__global" displayName="_e_geo__global" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="geo"/>
-    <tableColumn id="2" name="geo.is.global"/>
-    <tableColumn id="3" name="geo.name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,19 +860,22 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="2" max="2" width="14.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -914,9 +893,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>